<commit_message>
Fixed limit-10 reading function to read all tabs
</commit_message>
<xml_diff>
--- a/InputFiles/TC02_Bento_Filter_Arm-B.xlsx
+++ b/InputFiles/TC02_Bento_Filter_Arm-B.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohilz2\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ED787C6-9334-49C3-82A9-F37B5944A1B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E2D7121-4EDE-46CB-8CCA-92CED49C3268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16354" yWindow="-4860" windowWidth="33120" windowHeight="18120" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="27523" yWindow="1089" windowWidth="13731" windowHeight="8828" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -143,7 +143,7 @@
  order By samp.sample_id ASC LIMIT 100</t>
   </si>
   <si>
-    <t>MATCH (ss:study_subject)
+    <t xml:space="preserve">MATCH (ss:study_subject)
 MATCH (ss)&lt;-[:sample_of_study_subject]-(sp)&lt;-[:file_of_sample]-(f)-[:file_of_laboratory_procedure]-&gt;(lp)
 WITH ss, collect(DISTINCT sp.sample_id) AS samples, collect(DISTINCT lp.laboratory_procedure_id) AS lab_procedures, collect(DISTINCT f) AS files
 MATCH (ss)-[:study_subject_of_study]-&gt;(s)-[:study_of_program]-&gt;(p)
@@ -163,7 +163,7 @@
        d.pr_status AS `PR Status`,
        demo.age_at_index AS `Age (years)`,
 demo.survival_time AS `Survival (days)`
- order By ss.study_subject_id ASC LIMIT 100</t>
+ order By ss.study_subject_id ASC LIMIT 100 </t>
   </si>
 </sst>
 </file>
@@ -536,7 +536,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>